<commit_message>
added the eastings and Northings
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="8955" windowHeight="6885" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="14460" windowHeight="8175" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,17 +16,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -56,9 +50,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -403,31 +396,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16.7109375" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="12.85546875" customWidth="1" min="4" max="4"/>
-    <col width="16.42578125" customWidth="1" min="5" max="5"/>
-    <col width="12.5703125" customWidth="1" min="6" max="6"/>
+    <col width="14.28515625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Station</t>
+          <t>Stns</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Observed Angles</t>
+          <t>Obs Angles</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -478,6 +466,16 @@
       <c r="L1" t="inlineStr">
         <is>
           <t>correctedLatitude</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Eastings</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Northings</t>
         </is>
       </c>
     </row>
@@ -488,38 +486,44 @@
         </is>
       </c>
       <c r="B2">
-        <f>(81)+(11/60)+(50/3600)</f>
+        <f>(86)+(30/60)+(2/3600)</f>
         <v/>
       </c>
       <c r="C2" t="n">
-        <v>155</v>
+        <v>187.4</v>
       </c>
       <c r="D2" t="n">
-        <v>0.002777777777782831</v>
+        <v>-0.0013888888888971</v>
       </c>
       <c r="E2" t="n">
-        <v>81.2</v>
+        <v>86.49916666666665</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>140.1944444444445</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>119.97</v>
       </c>
       <c r="H2" t="n">
-        <v>155</v>
+        <v>-143.96</v>
       </c>
       <c r="I2" t="n">
-        <v>0.06880548829701515</v>
+        <v>-0.007200768491838459</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1038337368845841</v>
+        <v>-0.00540057636887117</v>
       </c>
       <c r="K2" t="n">
-        <v>0.06880548829701515</v>
+        <v>119.9627992315082</v>
       </c>
       <c r="L2" t="n">
-        <v>155.1038337368846</v>
+        <v>-143.9654005763689</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="3">
@@ -529,38 +533,44 @@
         </is>
       </c>
       <c r="B3">
-        <f>(120)+(25/60)+(50/3600)</f>
+        <f>(80)+(59/60)+(34/3600)</f>
         <v/>
       </c>
       <c r="C3" t="n">
-        <v>200</v>
+        <v>382.7</v>
       </c>
       <c r="D3" t="n">
-        <v>0.002777777777782831</v>
+        <v>-0.0013888888888971</v>
       </c>
       <c r="E3" t="n">
-        <v>120.4333333333333</v>
+        <v>80.99138888888888</v>
       </c>
       <c r="F3" t="n">
-        <v>300.4333333333333</v>
+        <v>41.18583333333333</v>
       </c>
       <c r="G3" t="n">
-        <v>-172.44</v>
+        <v>252.01</v>
       </c>
       <c r="H3" t="n">
-        <v>101.31</v>
+        <v>288.01</v>
       </c>
       <c r="I3" t="n">
-        <v>0.08878127522195502</v>
+        <v>-0.0147050912584129</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1339790153349472</v>
+        <v>-0.011028818443794</v>
       </c>
       <c r="K3" t="n">
-        <v>-172.3512187247781</v>
+        <v>251.9952949087416</v>
       </c>
       <c r="L3" t="n">
-        <v>101.4439790153349</v>
+        <v>287.9989711815562</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1119.96</v>
+      </c>
+      <c r="N3" t="n">
+        <v>856.03</v>
       </c>
     </row>
     <row r="4">
@@ -570,38 +580,44 @@
         </is>
       </c>
       <c r="B4">
-        <f>(149)+(33/60)+(50/3600)</f>
+        <f>(91)+(31/60)+(29/3600)</f>
         <v/>
       </c>
       <c r="C4" t="n">
-        <v>249</v>
+        <v>106.1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.002777777777782831</v>
+        <v>-0.0013888888888971</v>
       </c>
       <c r="E4" t="n">
-        <v>149.5666666666667</v>
+        <v>91.52333333333333</v>
       </c>
       <c r="F4" t="n">
-        <v>270</v>
+        <v>312.7091666666666</v>
       </c>
       <c r="G4" t="n">
-        <v>-249</v>
+        <v>-77.95999999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>-0</v>
+        <v>71.97</v>
       </c>
       <c r="I4" t="n">
-        <v>0.110532687651334</v>
+        <v>-0.004076849183479511</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1668038740920093</v>
+        <v>-0.003057636887605288</v>
       </c>
       <c r="K4" t="n">
-        <v>-248.8894673123487</v>
+        <v>-77.96407684918347</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1668038740920093</v>
+        <v>71.96694236311239</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1371.96</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1144.03</v>
       </c>
     </row>
     <row r="5">
@@ -611,135 +627,107 @@
         </is>
       </c>
       <c r="B5">
-        <f>95+(41/60)+(50/3600)</f>
+        <f>(100)+(59/60)+(15/3600)</f>
         <v/>
       </c>
       <c r="C5" t="n">
-        <v>190</v>
+        <v>364.8</v>
       </c>
       <c r="D5" t="n">
-        <v>0.002777777777782831</v>
+        <v>-0.0013888888888971</v>
       </c>
       <c r="E5" t="n">
-        <v>95.7</v>
+        <v>100.9861111111111</v>
       </c>
       <c r="F5" t="n">
-        <v>185.7</v>
+        <v>233.6952777777777</v>
       </c>
       <c r="G5" t="n">
-        <v>-18.87</v>
+        <v>-293.98</v>
       </c>
       <c r="H5" t="n">
-        <v>-189.06</v>
+        <v>-215.99</v>
       </c>
       <c r="I5" t="n">
-        <v>0.08434221146085727</v>
+        <v>-0.01401729106628959</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1272800645681999</v>
+        <v>-0.01051296829970225</v>
       </c>
       <c r="K5" t="n">
-        <v>-18.78565778853914</v>
+        <v>-293.9940172910663</v>
       </c>
       <c r="L5" t="n">
-        <v>-188.9327199354318</v>
+        <v>-216.0005129682997</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1294</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1216</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="B6">
-        <f>93+(5/60)+(50/3600)</f>
-        <v/>
-      </c>
-      <c r="C6" t="n">
-        <v>445</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.002777777777782831</v>
-      </c>
-      <c r="E6" t="n">
-        <v>93.09999999999999</v>
-      </c>
-      <c r="F6" t="n">
-        <v>98.80000000000007</v>
-      </c>
-      <c r="G6" t="n">
-        <v>439.76</v>
-      </c>
-      <c r="H6" t="n">
-        <v>-68.08</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.1975383373688499</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.2981033091202576</v>
-      </c>
-      <c r="K6" t="n">
-        <v>439.9575383373688</v>
-      </c>
-      <c r="L6" t="n">
-        <v>-67.78189669087973</v>
+      <c r="F6" s="1" t="n">
+        <v>140.1944444444444</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>1000.01</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="7">
-      <c r="F7" s="2" t="n">
-        <v>5.684341886080801e-14</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>360.0055555555556</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1041</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.005555555555588398</v>
+      </c>
+      <c r="E7" t="n">
+        <v>360</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.04000000000002046</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.02999999999997272</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-0.04000000000002046</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-0.02999999999997271</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>539.9861111111111</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1239</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.01388888888891415</v>
-      </c>
-      <c r="E8" t="n">
-        <v>540</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-0.5500000000000114</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-0.8299999999999983</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.5500000000000114</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.8299999999999983</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 / 1245</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="1" t="n"/>
+          <t>Fractional Misclosure</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1 / 20820</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>